<commit_message>
Updated migration with groups start date
</commit_message>
<xml_diff>
--- a/ChurchManager.DataImporter/churchmanager_db_data_import.xlsx
+++ b/ChurchManager.DataImporter/churchmanager_db_data_import.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Development\Freelance\ChurchManager\ChurchManager.DataImporter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35A69198-AE0D-48FC-B03B-D70F11B0789C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8592A25-F740-40E4-A985-66C630924405}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="47988" yWindow="12" windowWidth="13440" windowHeight="16656" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="384" yWindow="384" windowWidth="21744" windowHeight="16656" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Churches" sheetId="4" r:id="rId1"/>
@@ -34,35 +34,20 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="88">
   <si>
     <t>FullName_Title</t>
   </si>
   <si>
-    <t>FullName_FirstName</t>
-  </si>
-  <si>
     <t>FullName_NickName</t>
   </si>
   <si>
     <t>FullName_MiddleName</t>
   </si>
   <si>
-    <t>FullName_LastName</t>
-  </si>
-  <si>
     <t>FullName_Suffix</t>
   </si>
   <si>
-    <t>ConnectionStatus</t>
-  </si>
-  <si>
-    <t>AgeClassification</t>
-  </si>
-  <si>
-    <t>Gender</t>
-  </si>
-  <si>
     <t>BirthDate_BirthDay</t>
   </si>
   <si>
@@ -150,9 +135,6 @@
     <t>Daniel</t>
   </si>
   <si>
-    <t>Family</t>
-  </si>
-  <si>
     <t>Cagnetta Family</t>
   </si>
   <si>
@@ -187,9 +169,6 @@
   </si>
   <si>
     <t>Cape Town</t>
-  </si>
-  <si>
-    <t>Name</t>
   </si>
   <si>
     <t>Address_Street</t>
@@ -378,6 +357,36 @@
   </si>
   <si>
     <t>0737378631</t>
+  </si>
+  <si>
+    <t>StartDate</t>
+  </si>
+  <si>
+    <t>Name*</t>
+  </si>
+  <si>
+    <t>Church*</t>
+  </si>
+  <si>
+    <t>Family*</t>
+  </si>
+  <si>
+    <t>FullName_FirstName*</t>
+  </si>
+  <si>
+    <t>FullName_LastName*</t>
+  </si>
+  <si>
+    <t>ConnectionStatus*</t>
+  </si>
+  <si>
+    <t>AgeClassification*</t>
+  </si>
+  <si>
+    <t>Gender*</t>
+  </si>
+  <si>
+    <t>PhoneNumber*</t>
   </si>
 </sst>
 </file>
@@ -904,7 +913,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="15" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="8" xfId="15" applyFont="1" applyFill="1"/>
@@ -915,10 +924,13 @@
     <xf numFmtId="14" fontId="0" fillId="8" borderId="8" xfId="15" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="36" borderId="8" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="35" borderId="8" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="8" xfId="15" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="8" xfId="15" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="34" borderId="8" xfId="15" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="16" fillId="35" borderId="8" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -1287,9 +1299,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7A93222-CD45-4D80-95E6-7C8911F33824}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1301,37 +1311,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>51</v>
+      <c r="A1" s="11" t="s">
+        <v>79</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="B2" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="C2" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="D2" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="E2" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -1342,10 +1352,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11FEC808-0006-41C7-AC50-7A5AD8BFCD1F}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1355,57 +1365,64 @@
     <col min="3" max="3" width="59.5546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.6640625" style="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>51</v>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="11" t="s">
+        <v>79</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F2" t="s">
+        <v>44</v>
+      </c>
+      <c r="G2" s="8">
+        <v>43831</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B3" t="s">
         <v>63</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>65</v>
-      </c>
-      <c r="B2" t="s">
-        <v>71</v>
-      </c>
-      <c r="C2" t="s">
-        <v>68</v>
-      </c>
-      <c r="D2" t="s">
-        <v>47</v>
-      </c>
-      <c r="F2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>69</v>
-      </c>
-      <c r="B3" t="s">
-        <v>70</v>
-      </c>
       <c r="E3" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="F3" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -1419,7 +1436,7 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Q10" sqref="Q10"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1434,54 +1451,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>51</v>
+      <c r="A1" s="11" t="s">
+        <v>79</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B2" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="C2" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="D2" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="E2" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="F2">
         <v>8040</v>
       </c>
       <c r="G2" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="H4" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
@@ -1498,8 +1515,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AD5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
-      <selection activeCell="X23" sqref="X23"/>
+    <sheetView tabSelected="1" topLeftCell="W1" workbookViewId="0">
+      <selection activeCell="AB2" sqref="AB2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1521,7 +1538,7 @@
     <col min="20" max="20" width="16.21875" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="11.88671875" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="14.44140625" style="11" customWidth="1"/>
+    <col min="23" max="23" width="14.44140625" style="10" customWidth="1"/>
     <col min="24" max="24" width="23.77734375" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="23.109375" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="76.88671875" bestFit="1" customWidth="1"/>
@@ -1532,118 +1549,118 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>38</v>
+      <c r="A1" s="11" t="s">
+        <v>81</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="H1" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="I1" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="J1" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="K1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="L1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="N1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="O1" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="P1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="Q1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="R1" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="S1" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="T1" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="U1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="7" t="s">
+      <c r="W1" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="X1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="Y1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="Z1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="R1" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="S1" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="T1" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="U1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="V1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="W1" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="X1" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="Y1" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="AB1" s="1" t="s">
-        <v>43</v>
+      <c r="AB1" s="11" t="s">
+        <v>80</v>
       </c>
       <c r="AC1" s="6" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="AD1" s="6" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B2" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C2" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="F2" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="H2" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="I2" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="J2" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="K2">
         <v>6</v>
@@ -1655,75 +1672,75 @@
         <v>1981</v>
       </c>
       <c r="N2" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="O2" s="8">
         <v>38144</v>
       </c>
       <c r="P2" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="R2" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="S2" s="8">
         <v>38509</v>
       </c>
       <c r="T2" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="U2" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="V2" s="8">
         <v>41275</v>
       </c>
-      <c r="W2" s="11" t="s">
-        <v>84</v>
+      <c r="W2" s="10" t="s">
+        <v>77</v>
       </c>
       <c r="X2" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="Y2" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="Z2" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="AA2" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="AB2" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="AC2" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="AD2" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B3" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C3" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="F3" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="H3" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="I3" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="J3" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="K3">
         <v>13</v>
@@ -1735,63 +1752,63 @@
         <v>1980</v>
       </c>
       <c r="N3" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="P3" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="R3" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="T3" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="U3" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="V3" s="8">
         <v>41275</v>
       </c>
       <c r="X3" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="Y3" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="Z3" t="s">
+        <v>29</v>
+      </c>
+      <c r="AA3" t="s">
         <v>34</v>
       </c>
-      <c r="AA3" t="s">
-        <v>40</v>
-      </c>
       <c r="AB3" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="AC3" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="AD3" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C4" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="F4" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="H4" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="I4" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="J4" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="K4">
         <v>6</v>
@@ -1803,42 +1820,42 @@
         <v>2017</v>
       </c>
       <c r="N4" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="P4" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="T4" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="AB4" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="AC4" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="AD4" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C5" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="F5" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="H5" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="I5" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="J5" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="K5">
         <v>28</v>
@@ -1850,13 +1867,13 @@
         <v>2013</v>
       </c>
       <c r="P5" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="T5" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="AB5" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated: import of groups
</commit_message>
<xml_diff>
--- a/ChurchManager.DataImporter/churchmanager_db_data_import.xlsx
+++ b/ChurchManager.DataImporter/churchmanager_db_data_import.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Development\Freelance\ChurchManager\ChurchManager.DataImporter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8592A25-F740-40E4-A985-66C630924405}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD521633-B05B-4A85-B1A1-EA662293E203}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="384" windowWidth="21744" windowHeight="16656" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="384" yWindow="384" windowWidth="21744" windowHeight="16656" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Churches" sheetId="4" r:id="rId1"/>
@@ -273,77 +273,6 @@
     <t>Cape Town Church</t>
   </si>
   <si>
-    <r>
-      <t>7 West Quay</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF4D5156"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>, </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="8"/>
-        <color rgb="FF5F6368"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>West Quay Road</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF4D5156"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>, </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="8"/>
-        <color rgb="FF5F6368"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Waterfront</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF4D5156"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>. </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="8"/>
-        <color rgb="FF5F6368"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Waterfront</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF4D5156"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>, Cape Town</t>
-    </r>
-  </si>
-  <si>
     <t>ShortCode</t>
   </si>
   <si>
@@ -353,9 +282,6 @@
     <t>PhoneNumber</t>
   </si>
   <si>
-    <t> 0214472004</t>
-  </si>
-  <si>
     <t>0737378631</t>
   </si>
   <si>
@@ -387,6 +313,12 @@
   </si>
   <si>
     <t>PhoneNumber*</t>
+  </si>
+  <si>
+    <t>0214472004</t>
+  </si>
+  <si>
+    <t>7 West Quay, West Quay Road, Waterfront. Waterfront, Cape Town</t>
   </si>
 </sst>
 </file>
@@ -913,7 +845,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="15" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="8" xfId="15" applyFont="1" applyFill="1"/>
@@ -933,6 +865,8 @@
     <xf numFmtId="49" fontId="16" fillId="35" borderId="8" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="8" borderId="8" xfId="15" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1299,7 +1233,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7A93222-CD45-4D80-95E6-7C8911F33824}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1307,12 +1243,12 @@
     <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="59.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" style="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>56</v>
@@ -1321,10 +1257,10 @@
         <v>60</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
+      </c>
+      <c r="E1" s="15" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -1335,13 +1271,13 @@
         <v>71</v>
       </c>
       <c r="C2" t="s">
-        <v>72</v>
+        <v>87</v>
       </c>
       <c r="D2" t="s">
-        <v>74</v>
-      </c>
-      <c r="E2" t="s">
-        <v>76</v>
+        <v>73</v>
+      </c>
+      <c r="E2" s="16" t="s">
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -1355,7 +1291,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1370,7 +1306,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>56</v>
@@ -1385,10 +1321,10 @@
         <v>59</v>
       </c>
       <c r="F1" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -1452,7 +1388,7 @@
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>45</v>
@@ -1515,7 +1451,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AD5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="W1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AB2" sqref="AB2"/>
     </sheetView>
   </sheetViews>
@@ -1550,13 +1486,13 @@
   <sheetData>
     <row r="1" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>1</v>
@@ -1565,19 +1501,19 @@
         <v>2</v>
       </c>
       <c r="F1" s="12" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="H1" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="I1" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="J1" s="13" t="s">
         <v>84</v>
-      </c>
-      <c r="I1" s="13" t="s">
-        <v>85</v>
-      </c>
-      <c r="J1" s="13" t="s">
-        <v>86</v>
       </c>
       <c r="K1" s="3" t="s">
         <v>4</v>
@@ -1616,7 +1552,7 @@
         <v>12</v>
       </c>
       <c r="W1" s="14" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="X1" s="4" t="s">
         <v>13</v>
@@ -1631,7 +1567,7 @@
         <v>16</v>
       </c>
       <c r="AB1" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="AC1" s="6" t="s">
         <v>65</v>
@@ -1696,7 +1632,7 @@
         <v>41275</v>
       </c>
       <c r="W2" s="10" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="X2" t="s">
         <v>23</v>

</xml_diff>

<commit_message>
Added: meeeting date time
</commit_message>
<xml_diff>
--- a/ChurchManager.DataImporter/churchmanager_db_data_import.xlsx
+++ b/ChurchManager.DataImporter/churchmanager_db_data_import.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Development\Freelance\ChurchManager\ChurchManager.DataImporter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1BDCEC6-3B9B-424D-BBD7-7A904701CC9D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BDADA78-827F-4545-96DB-F05D6BB7499E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="384" windowWidth="21744" windowHeight="16656" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="21768" yWindow="12" windowWidth="26208" windowHeight="16656" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Churches" sheetId="4" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="97">
   <si>
     <t>FullName_Title</t>
   </si>
@@ -332,12 +332,27 @@
   <si>
     <t>Split from the parent also</t>
   </si>
+  <si>
+    <t>Thursday</t>
+  </si>
+  <si>
+    <t>Friday</t>
+  </si>
+  <si>
+    <t>Saturday</t>
+  </si>
+  <si>
+    <t>MeetingDay*</t>
+  </si>
+  <si>
+    <t>MeetingTime*</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -484,6 +499,12 @@
       <color rgb="FF5F6368"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="40">
@@ -869,7 +890,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="15" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="8" xfId="15" applyFont="1" applyFill="1"/>
@@ -893,6 +914,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="38" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="39" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1314,10 +1336,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11FEC808-0006-41C7-AC50-7A5AD8BFCD1F}">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1328,9 +1350,11 @@
     <col min="5" max="5" width="21.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.6640625" style="8" customWidth="1"/>
+    <col min="8" max="8" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
         <v>77</v>
       </c>
@@ -1352,8 +1376,14 @@
       <c r="G1" s="7" t="s">
         <v>76</v>
       </c>
+      <c r="H1" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="I1" s="11" t="s">
+        <v>96</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="17" t="s">
         <v>58</v>
       </c>
@@ -1372,8 +1402,14 @@
       <c r="G2" s="8">
         <v>43831</v>
       </c>
+      <c r="H2" t="s">
+        <v>92</v>
+      </c>
+      <c r="I2" s="19">
+        <v>0.58333333333333337</v>
+      </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="18" t="s">
         <v>62</v>
       </c>
@@ -1386,8 +1422,14 @@
       <c r="F3" t="s">
         <v>44</v>
       </c>
+      <c r="H3" t="s">
+        <v>93</v>
+      </c>
+      <c r="I3" s="19">
+        <v>0.625</v>
+      </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>90</v>
       </c>
@@ -1400,8 +1442,14 @@
       <c r="F4" t="s">
         <v>44</v>
       </c>
+      <c r="H4" t="s">
+        <v>94</v>
+      </c>
+      <c r="I4" s="19">
+        <v>0.58333333333333337</v>
+      </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>88</v>
       </c>
@@ -1417,8 +1465,15 @@
       <c r="F5" t="s">
         <v>44</v>
       </c>
+      <c r="H5" t="s">
+        <v>92</v>
+      </c>
+      <c r="I5" s="19">
+        <v>0.70833333333333304</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="20" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated: migrations and added group tree creator
</commit_message>
<xml_diff>
--- a/ChurchManager.DataImporter/churchmanager_db_data_import.xlsx
+++ b/ChurchManager.DataImporter/churchmanager_db_data_import.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Development\Freelance\ChurchManager\ChurchManager.DataImporter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04D65228-F526-4365-88C6-4D471B8EA5C9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F77CBB38-65DE-41F7-83C8-84A7C2DA1B01}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="21768" yWindow="12" windowWidth="26208" windowHeight="16656" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1348,7 +1348,7 @@
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>